<commit_message>
Unified dataframe field handling, and take the schema override into account
</commit_message>
<xml_diff>
--- a/crates/geo/tests/data/data_types.xlsx
+++ b/crates/geo/tests/data/data_types.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07B78460-F2D5-4A1D-9297-AADE72972A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Projects/infra-rs/crates/geo/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63E539C-F3F1-A941-AB8F-DB4551DAE735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>String Column</t>
   </si>
@@ -55,6 +60,9 @@
   </si>
   <si>
     <t>Dana</t>
+  </si>
+  <si>
+    <t>Bool Column</t>
   </si>
 </sst>
 </file>
@@ -62,9 +70,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,7 +104,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,20 +407,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +434,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -439,8 +451,11 @@
       <c r="D2" s="2">
         <v>45063</v>
       </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -450,8 +465,11 @@
       <c r="D3" s="2">
         <v>44920</v>
       </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>45.67</v>
       </c>
@@ -461,8 +479,11 @@
       <c r="D4" s="2">
         <v>45292</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -473,7 +494,7 @@
         <v>44381</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -482,6 +503,9 @@
       </c>
       <c r="C6" s="1">
         <v>56</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>